<commit_message>
Gå tillbaka till main menu
</commit_message>
<xml_diff>
--- a/Dokumentation/Iteration v17/Iteration 2.xlsx
+++ b/Dokumentation/Iteration v17/Iteration 2.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Analys av föregående iteration</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Denna iteration hann jag faktiskt inte med allting som jag hade planerat eftersom jag har en tendens att skjuta upp saker. Det är alltid svårt att börja och det var det som jag sköt upp på hela tiden och har därför hamnat efter i planeringen. Att implementera state management tog lyckligtvis inte så långt tid som jag trodde och kunde då börja på min meny. Menyn verkar ta rätt långt tid då jag inte ens hann färdigt på de 6 timmar jag trodde det skulle ta. Därför får jag flytta över det till nästa iteration.  Jag lyckades inte heller göra någon testning så jag får göra det nästa iteration istället.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tankar och funderingar </t>
+  </si>
+  <si>
+    <t>Pågående</t>
   </si>
 </sst>
 </file>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,12 +834,14 @@
         <v>30</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D28" s="4">
         <v>1.5</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -860,12 +868,14 @@
         <v>34</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D30" s="4">
         <v>1.5</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -925,36 +935,55 @@
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4" t="s">
-        <v>8</v>
+      <c r="B35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="D35" s="4">
-        <v>22.5</v>
-      </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E35" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="7" t="s">
-        <v>9</v>
+      <c r="C36" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D36" s="4">
-        <v>47.5</v>
+        <f>SUM(D24:D35)</f>
+        <v>28.5</v>
       </c>
       <c r="E36" s="4">
-        <v>41.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <f>SUM(E24:E35)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="4">
+        <v>47.5</v>
+      </c>
+      <c r="E37" s="4">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Platta, testning med testrapport
</commit_message>
<xml_diff>
--- a/Dokumentation/Iteration v17/Iteration 2.xlsx
+++ b/Dokumentation/Iteration v17/Iteration 2.xlsx
@@ -136,16 +136,16 @@
     <t>Funktioner för att styra plattan med musen</t>
   </si>
   <si>
-    <t>Testfall</t>
-  </si>
-  <si>
     <t>Denna iteration hann jag faktiskt inte med allting som jag hade planerat eftersom jag har en tendens att skjuta upp saker. Det är alltid svårt att börja och det var det som jag sköt upp på hela tiden och har därför hamnat efter i planeringen. Att implementera state management tog lyckligtvis inte så långt tid som jag trodde och kunde då börja på min meny. Menyn verkar ta rätt långt tid då jag inte ens hann färdigt på de 6 timmar jag trodde det skulle ta. Därför får jag flytta över det till nästa iteration.  Jag lyckades inte heller göra någon testning så jag får göra det nästa iteration istället.</t>
   </si>
   <si>
-    <t xml:space="preserve">Tankar och funderingar </t>
-  </si>
-  <si>
-    <t>Pågående</t>
+    <t>Tankar och funderingar</t>
+  </si>
+  <si>
+    <t>Testspecifikation och testfall</t>
+  </si>
+  <si>
+    <t>Testning och testrapport</t>
   </si>
 </sst>
 </file>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,8 +537,8 @@
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -885,12 +885,14 @@
         <v>37</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D31" s="4">
         <v>4</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -900,52 +902,58 @@
         <v>39</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D32" s="4">
         <v>3</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D33" s="4">
         <v>3</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D34" s="4">
         <v>2</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D35" s="4">
         <v>6</v>
       </c>
       <c r="E35" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -960,7 +968,7 @@
       </c>
       <c r="E36" s="4">
         <f>SUM(E24:E35)</f>
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>